<commit_message>
Now boasts data before 2014 as well!
</commit_message>
<xml_diff>
--- a/output/AGO.xlsx
+++ b/output/AGO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,27 +456,47 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>4. Agriculture land area (% of land area)</t>
+          <t>4. Agriculture land area (% of land area)_x</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>4. Agriculture land area (% of land area)_y</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>5. Average precipitation (mm)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>7. Fertilizer consumption (kilograms per hectare of arable land)</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>13. Population</t>
+          <t>7. Fertilizer consumption (kilograms per hectare of arable land)_x</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>17. Employment in agriculture (% of total employment) (modeled ILO estimate)</t>
+          <t>7. Fertilizer consumption (kilograms per hectare of arable land)_y</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>13. Population_x</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>13. Population_y</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>17. Employment in agriculture (% of total employment) (modeled ILO estimate)_x</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>17. Employment in agriculture (% of total employment) (modeled ILO estimate)_y</t>
         </is>
       </c>
     </row>
@@ -487,29 +507,1031 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>1991</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>13.8</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>22.44</v>
+      </c>
+      <c r="E2" t="n">
+        <v>35.68059678</v>
+      </c>
+      <c r="F2" t="n">
+        <v>35.68059678</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1107.7</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.338983051</v>
+      </c>
+      <c r="I2" t="n">
+        <v>2.338983051</v>
+      </c>
+      <c r="J2" t="n">
+        <v>12228691</v>
+      </c>
+      <c r="K2" t="n">
+        <v>12228691</v>
+      </c>
+      <c r="L2" t="n">
+        <v>40.0718566747821</v>
+      </c>
+      <c r="M2" t="n">
+        <v>40.0718566747821</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1992</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>14.79</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>22.02</v>
+      </c>
+      <c r="E3" t="n">
+        <v>35.70305607</v>
+      </c>
+      <c r="F3" t="n">
+        <v>35.70305607</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1121.29</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3.033333333</v>
+      </c>
+      <c r="I3" t="n">
+        <v>3.033333333</v>
+      </c>
+      <c r="J3" t="n">
+        <v>12632507</v>
+      </c>
+      <c r="K3" t="n">
+        <v>12632507</v>
+      </c>
+      <c r="L3" t="n">
+        <v>39.9382622594256</v>
+      </c>
+      <c r="M3" t="n">
+        <v>39.9382622594256</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1993</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>14.72</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>22.1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>35.70225395</v>
+      </c>
+      <c r="F4" t="n">
+        <v>35.70225395</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1099.18</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2.666666667</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.666666667</v>
+      </c>
+      <c r="J4" t="n">
+        <v>13038270</v>
+      </c>
+      <c r="K4" t="n">
+        <v>13038270</v>
+      </c>
+      <c r="L4" t="n">
+        <v>40.1263803076634</v>
+      </c>
+      <c r="M4" t="n">
+        <v>40.1263803076634</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1994</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>18.03</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>22.31</v>
+      </c>
+      <c r="E5" t="n">
+        <v>35.70225395</v>
+      </c>
+      <c r="F5" t="n">
+        <v>35.70225395</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1163.07</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3.333333333</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3.333333333</v>
+      </c>
+      <c r="J5" t="n">
+        <v>13462031</v>
+      </c>
+      <c r="K5" t="n">
+        <v>13462031</v>
+      </c>
+      <c r="L5" t="n">
+        <v>39.891772320315</v>
+      </c>
+      <c r="M5" t="n">
+        <v>39.891772320315</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1995</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>18.06</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>22.37</v>
+      </c>
+      <c r="E6" t="n">
+        <v>35.6862116</v>
+      </c>
+      <c r="F6" t="n">
+        <v>35.6862116</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1132.65</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2.666666667</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2.666666667</v>
+      </c>
+      <c r="J6" t="n">
+        <v>13912253</v>
+      </c>
+      <c r="K6" t="n">
+        <v>13912253</v>
+      </c>
+      <c r="L6" t="n">
+        <v>39.3849532691177</v>
+      </c>
+      <c r="M6" t="n">
+        <v>39.3849532691177</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1996</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>18.54</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>22.34</v>
+      </c>
+      <c r="E7" t="n">
+        <v>35.65172054</v>
+      </c>
+      <c r="F7" t="n">
+        <v>35.65172054</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1181.38</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" t="n">
+        <v>14383350</v>
+      </c>
+      <c r="K7" t="n">
+        <v>14383350</v>
+      </c>
+      <c r="L7" t="n">
+        <v>38.8025436477442</v>
+      </c>
+      <c r="M7" t="n">
+        <v>38.8025436477442</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1997</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>18.07</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>35.6541269</v>
+      </c>
+      <c r="F8" t="n">
+        <v>35.6541269</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1146.17</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.666666667</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.666666667</v>
+      </c>
+      <c r="J8" t="n">
+        <v>14871146</v>
+      </c>
+      <c r="K8" t="n">
+        <v>14871146</v>
+      </c>
+      <c r="L8" t="n">
+        <v>38.4197642709686</v>
+      </c>
+      <c r="M8" t="n">
+        <v>38.4197642709686</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1998</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>21.99</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>22.58</v>
+      </c>
+      <c r="E9" t="n">
+        <v>35.7046603</v>
+      </c>
+      <c r="F9" t="n">
+        <v>35.7046603</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1136.75</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.133333333</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.133333333</v>
+      </c>
+      <c r="J9" t="n">
+        <v>15366864</v>
+      </c>
+      <c r="K9" t="n">
+        <v>15366864</v>
+      </c>
+      <c r="L9" t="n">
+        <v>38.1697504172627</v>
+      </c>
+      <c r="M9" t="n">
+        <v>38.1697504172627</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1999</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>20.9</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>22.53</v>
+      </c>
+      <c r="E10" t="n">
+        <v>35.74797465</v>
+      </c>
+      <c r="F10" t="n">
+        <v>35.74797465</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1132.97</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.133333333</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.133333333</v>
+      </c>
+      <c r="J10" t="n">
+        <v>15870753</v>
+      </c>
+      <c r="K10" t="n">
+        <v>15870753</v>
+      </c>
+      <c r="L10" t="n">
+        <v>37.572139586702</v>
+      </c>
+      <c r="M10" t="n">
+        <v>37.572139586702</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>25.49</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>22.59</v>
+      </c>
+      <c r="E11" t="n">
+        <v>35.71268148</v>
+      </c>
+      <c r="F11" t="n">
+        <v>35.71268148</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1146.88</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.466666667</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.466666667</v>
+      </c>
+      <c r="J11" t="n">
+        <v>16394062</v>
+      </c>
+      <c r="K11" t="n">
+        <v>16394062</v>
+      </c>
+      <c r="L11" t="n">
+        <v>37.1460067373979</v>
+      </c>
+      <c r="M11" t="n">
+        <v>37.1460067373979</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2002</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>36.2</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>22.67</v>
+      </c>
+      <c r="E12" t="n">
+        <v>35.64450148</v>
+      </c>
+      <c r="F12" t="n">
+        <v>35.64450148</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1107.55</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.659032258</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.659032258</v>
+      </c>
+      <c r="J12" t="n">
+        <v>17516139</v>
+      </c>
+      <c r="K12" t="n">
+        <v>17516139</v>
+      </c>
+      <c r="L12" t="n">
+        <v>36.4258485038886</v>
+      </c>
+      <c r="M12" t="n">
+        <v>36.4258485038886</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2003</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>40.15</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>22.72</v>
+      </c>
+      <c r="E13" t="n">
+        <v>35.69343066</v>
+      </c>
+      <c r="F13" t="n">
+        <v>35.69343066</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1144.58</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.788787879</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.788787879</v>
+      </c>
+      <c r="J13" t="n">
+        <v>18124342</v>
+      </c>
+      <c r="K13" t="n">
+        <v>18124342</v>
+      </c>
+      <c r="L13" t="n">
+        <v>36.1555716487064</v>
+      </c>
+      <c r="M13" t="n">
+        <v>36.1555716487064</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2004</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>45.52</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>22.84</v>
+      </c>
+      <c r="E14" t="n">
+        <v>35.54183043</v>
+      </c>
+      <c r="F14" t="n">
+        <v>35.54183043</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1132.41</v>
+      </c>
+      <c r="H14" t="n">
+        <v>4.501515152</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4.501515152</v>
+      </c>
+      <c r="J14" t="n">
+        <v>18771125</v>
+      </c>
+      <c r="K14" t="n">
+        <v>18771125</v>
+      </c>
+      <c r="L14" t="n">
+        <v>36.1663353037515</v>
+      </c>
+      <c r="M14" t="n">
+        <v>36.1663353037515</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2005</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>49.15</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>22.66</v>
+      </c>
+      <c r="E15" t="n">
+        <v>35.4399615</v>
+      </c>
+      <c r="F15" t="n">
+        <v>35.4399615</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1133.78</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2.260606061</v>
+      </c>
+      <c r="I15" t="n">
+        <v>2.260606061</v>
+      </c>
+      <c r="J15" t="n">
+        <v>19450959</v>
+      </c>
+      <c r="K15" t="n">
+        <v>19450959</v>
+      </c>
+      <c r="L15" t="n">
+        <v>38.1609804036611</v>
+      </c>
+      <c r="M15" t="n">
+        <v>38.1609804036611</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2006</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>50.36</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>22.64</v>
+      </c>
+      <c r="E16" t="n">
+        <v>35.40306409</v>
+      </c>
+      <c r="F16" t="n">
+        <v>35.40306409</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1132.27</v>
+      </c>
+      <c r="H16" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="I16" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="J16" t="n">
+        <v>20162340</v>
+      </c>
+      <c r="K16" t="n">
+        <v>20162340</v>
+      </c>
+      <c r="L16" t="n">
+        <v>40.5238640648733</v>
+      </c>
+      <c r="M16" t="n">
+        <v>40.5238640648733</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>58.33</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>22.68</v>
+      </c>
+      <c r="E17" t="n">
+        <v>35.48969279</v>
+      </c>
+      <c r="F17" t="n">
+        <v>35.48969279</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1136.93</v>
+      </c>
+      <c r="H17" t="n">
+        <v>3.305</v>
+      </c>
+      <c r="I17" t="n">
+        <v>3.305</v>
+      </c>
+      <c r="J17" t="n">
+        <v>20909684</v>
+      </c>
+      <c r="K17" t="n">
+        <v>20909684</v>
+      </c>
+      <c r="L17" t="n">
+        <v>42.6903205223285</v>
+      </c>
+      <c r="M17" t="n">
+        <v>42.6903205223285</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>62.17</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>22.74</v>
+      </c>
+      <c r="E18" t="n">
+        <v>35.44958691</v>
+      </c>
+      <c r="F18" t="n">
+        <v>35.44958691</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1125.95</v>
+      </c>
+      <c r="H18" t="n">
+        <v>8.258823529000001</v>
+      </c>
+      <c r="I18" t="n">
+        <v>8.258823529000001</v>
+      </c>
+      <c r="J18" t="n">
+        <v>21691522</v>
+      </c>
+      <c r="K18" t="n">
+        <v>21691522</v>
+      </c>
+      <c r="L18" t="n">
+        <v>44.9381526016078</v>
+      </c>
+      <c r="M18" t="n">
+        <v>44.9381526016078</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>81.2</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>22.77</v>
+      </c>
+      <c r="E19" t="n">
+        <v>35.79850806</v>
+      </c>
+      <c r="F19" t="n">
+        <v>35.79850806</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1134.11</v>
+      </c>
+      <c r="H19" t="n">
+        <v>5.47225</v>
+      </c>
+      <c r="I19" t="n">
+        <v>5.47225</v>
+      </c>
+      <c r="J19" t="n">
+        <v>22507674</v>
+      </c>
+      <c r="K19" t="n">
+        <v>22507674</v>
+      </c>
+      <c r="L19" t="n">
+        <v>47.2185489495172</v>
+      </c>
+      <c r="M19" t="n">
+        <v>47.2185489495172</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>86.14</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>22.78</v>
+      </c>
+      <c r="E20" t="n">
+        <v>35.97497393</v>
+      </c>
+      <c r="F20" t="n">
+        <v>35.97497393</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1150.38</v>
+      </c>
+      <c r="H20" t="n">
+        <v>8.229285714</v>
+      </c>
+      <c r="I20" t="n">
+        <v>8.229285714</v>
+      </c>
+      <c r="J20" t="n">
+        <v>23364185</v>
+      </c>
+      <c r="K20" t="n">
+        <v>23364185</v>
+      </c>
+      <c r="L20" t="n">
+        <v>48.6825181321233</v>
+      </c>
+      <c r="M20" t="n">
+        <v>48.6825181321233</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>95.31</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>22.81</v>
+      </c>
+      <c r="E21" t="n">
+        <v>36.34876073</v>
+      </c>
+      <c r="F21" t="n">
+        <v>36.34876073</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1118.83</v>
+      </c>
+      <c r="H21" t="n">
+        <v>11.98382979</v>
+      </c>
+      <c r="I21" t="n">
+        <v>11.98382979</v>
+      </c>
+      <c r="J21" t="n">
+        <v>24259111</v>
+      </c>
+      <c r="K21" t="n">
+        <v>24259111</v>
+      </c>
+      <c r="L21" t="n">
+        <v>51.1022140863603</v>
+      </c>
+      <c r="M21" t="n">
+        <v>51.1022140863603</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>76.61</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>22.92</v>
+      </c>
+      <c r="E22" t="n">
+        <v>36.3383332</v>
+      </c>
+      <c r="F22" t="n">
+        <v>36.3383332</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1141.86</v>
+      </c>
+      <c r="H22" t="n">
+        <v>8.876048936</v>
+      </c>
+      <c r="I22" t="n">
+        <v>8.876048936</v>
+      </c>
+      <c r="J22" t="n">
+        <v>25188292</v>
+      </c>
+      <c r="K22" t="n">
+        <v>25188292</v>
+      </c>
+      <c r="L22" t="n">
+        <v>53.2924848831765</v>
+      </c>
+      <c r="M22" t="n">
+        <v>53.2924848831765</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>108.18</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="E23" t="n">
+        <v>36.48672495</v>
+      </c>
+      <c r="F23" t="n">
+        <v>36.48672495</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1127.39</v>
+      </c>
+      <c r="H23" t="n">
+        <v>9.369120743</v>
+      </c>
+      <c r="I23" t="n">
+        <v>9.369120743</v>
+      </c>
+      <c r="J23" t="n">
+        <v>26147002</v>
+      </c>
+      <c r="K23" t="n">
+        <v>26147002</v>
+      </c>
+      <c r="L23" t="n">
+        <v>55.4400666745874</v>
+      </c>
+      <c r="M23" t="n">
+        <v>55.4400666745874</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>AGO</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
         <v>2014</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>94</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D24" t="n">
         <v>22.87</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E24" t="n">
         <v>36.63591883</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F24" t="n">
+        <v>36.63591883</v>
+      </c>
+      <c r="G24" t="n">
         <v>1145.05</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H24" t="n">
         <v>9.056087824</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I24" t="n">
+        <v>9.056087824</v>
+      </c>
+      <c r="J24" t="n">
         <v>27128337</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K24" t="n">
+        <v>27128337</v>
+      </c>
+      <c r="L24" t="n">
+        <v>57.5996382189249</v>
+      </c>
+      <c r="M24" t="n">
         <v>57.5996382189249</v>
       </c>
     </row>

</xml_diff>